<commit_message>
fixing the build to generate jslint erros/warnings
</commit_message>
<xml_diff>
--- a/projects/WebUI/docs/issues.xlsx
+++ b/projects/WebUI/docs/issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>No</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Externalize the strings</t>
+  </si>
+  <si>
+    <t>Fixed</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +505,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>